<commit_message>
data and reports examples
</commit_message>
<xml_diff>
--- a/test_data/REPORT_test_data/Total_Results.xlsx
+++ b/test_data/REPORT_test_data/Total_Results.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="121" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
     <col width="39" customWidth="1" min="3" max="3"/>
     <col width="17" customWidth="1" min="4" max="4"/>
@@ -515,15 +515,15 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>MOCK_DATA.xlsx</t>
+          <t>MOCK_DATA_old - Copy here is very big name of the file, what can extend the total table.xlsx, file missed: NOT EXECUTED</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>['extra_sheet'] missing: NOT EXECUTED</t>
+          <t>NONE</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
@@ -551,61 +551,61 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>MOCK_DATA.xlsx</t>
+          <t>MOCK_DATA_old.xlsx, file missed: NOT EXECUTED</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>mock_data</t>
+          <t>NONE</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>152</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>144</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" s="3" t="n">
-        <v>114.00421</v>
-      </c>
-      <c r="J3" s="3" t="n">
-        <v>70</v>
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>MOCK_DATA.xlsx</t>
+          <t>MOCK_DATA_old_csv.csv, file missed: NOT EXECUTED</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>some_data</t>
+          <t>NONE</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>49</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>49</v>
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="G4" s="4" t="n">
         <v>0</v>
@@ -623,69 +623,285 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>MOCK_DATA.csv</t>
+          <t>banana_quality_dataset.xlsx</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>sheet</t>
+          <t>banana_quality_dataset.csv</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>150</v>
+        <v>976</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="G5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4" t="n">
-        <v>0</v>
+        <v>967</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>-2343.4462</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>2210</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>TOTAL</t>
+          <t>MOCK_DATA - csv.csv</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="inlineStr"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>sheet</t>
+        </is>
+      </c>
       <c r="D6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>144</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>351</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>343</v>
-      </c>
-      <c r="G6" s="3" t="n">
+      <c r="H6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>-31671.00874</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>31190</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Test_500_without big number.xlsx</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>MOCK_DATA (1).csv</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>504</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>493</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>5088</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>MOCK_DATA.xlsx</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>['extra_sheet'] missing: NOT EXECUTED</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>MOCK_DATA.xlsx</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>some_data</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>45.95812</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>MOCK_DATA.xlsx</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>mock_data</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>144</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3" t="n">
         <v>114.00421</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J10" s="3" t="n">
         <v>70</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Test_500.xlsx</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>MOCK_DATA (1).csv</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>502</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>494</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>665488751</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>730893583</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="inlineStr"/>
+      <c r="D12" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>2335</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>2288</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>665459984.50739</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>730893583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>